<commit_message>
commit as of 30/3/2020
</commit_message>
<xml_diff>
--- a/ocms/src/test/resources/DownloadedFiles/Wait Time Color Config.xlsx
+++ b/ocms/src/test/resources/DownloadedFiles/Wait Time Color Config.xlsx
@@ -169,10 +169,10 @@
     <t xml:space="preserve">08:59:00</t>
   </si>
   <si>
-    <t xml:space="preserve">#673262</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12/03/2020 19:31:22</t>
+    <t xml:space="preserve">#1e0e16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17/03/2020 00:05:33</t>
   </si>
   <si>
     <t xml:space="preserve">02:22:00</t>

</xml_diff>